<commit_message>
BackEnd Testing Added to Framework
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/CucumberTestData.xlsx
+++ b/src/test/resources/testdata/CucumberTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcbel\IdeaProjects\CucumberFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945F08E0-C843-4CAE-864D-8DCCB299F9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B919B84-4C5A-42F9-B6AE-531270177184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27810" yWindow="3045" windowWidth="18900" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25080" yWindow="1395" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EmployeeData" sheetId="1" r:id="rId1"/>
@@ -75,28 +75,28 @@
     <t>C:\Users\pcbel\Downloads\pic.jpg</t>
   </si>
   <si>
-    <t>Sarı895</t>
-  </si>
-  <si>
-    <t>Ali45ppda74</t>
-  </si>
-  <si>
-    <t>Suden1122</t>
-  </si>
-  <si>
-    <t>Saffa86522</t>
-  </si>
-  <si>
-    <t>alippli1236823</t>
-  </si>
-  <si>
-    <t>dedesırrı123523</t>
-  </si>
-  <si>
-    <t>sden1234223</t>
-  </si>
-  <si>
-    <t>Saraa1231123</t>
+    <t>Alida74</t>
+  </si>
+  <si>
+    <t>S954</t>
+  </si>
+  <si>
+    <t>S1122</t>
+  </si>
+  <si>
+    <t>Sa522</t>
+  </si>
+  <si>
+    <t>alippli236823</t>
+  </si>
+  <si>
+    <t>desırrı123523</t>
+  </si>
+  <si>
+    <t>sde234223</t>
+  </si>
+  <si>
+    <t>Saa1231123</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -494,7 +494,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>

</xml_diff>